<commit_message>
Kreuzmessung Versuch mit Fehlern
</commit_message>
<xml_diff>
--- a/Messprotokoll.xlsx
+++ b/Messprotokoll.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F54B412C-97E7-4439-AF16-2B133035DB64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB6DD71-B9F0-4C04-BB3A-DD3980869346}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3015" yWindow="4343" windowWidth="16875" windowHeight="10522" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="38">
   <si>
     <t>Simon Keegan, Philipp Gebauer</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t>S_Kreuz_Az-16Al00</t>
+  </si>
+  <si>
+    <t>fgs</t>
   </si>
 </sst>
 </file>
@@ -252,7 +255,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -532,33 +535,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B23" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="H73" sqref="H73"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="M61" sqref="M61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.19921875" customWidth="1"/>
+    <col min="1" max="1" width="10.21875" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.06640625" customWidth="1"/>
-    <col min="5" max="5" width="12.265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.53125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.19921875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.53125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.86328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.53125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.53125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.265625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.53125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.109375" customWidth="1"/>
+    <col min="5" max="5" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29" customWidth="1"/>
+    <col min="9" max="9" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -566,27 +569,27 @@
         <v>43964</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>1410</v>
       </c>
@@ -595,7 +598,7 @@
       </c>
       <c r="H7" s="11"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>4</v>
       </c>
@@ -621,7 +624,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <v>0.35391203703703705</v>
       </c>
@@ -644,7 +647,7 @@
         <v>308.3</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <v>0.35440972222222222</v>
       </c>
@@ -664,7 +667,7 @@
         <v>318.5</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <v>0.35487268518518517</v>
       </c>
@@ -684,7 +687,7 @@
         <v>324.8</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="9">
         <v>0.3552777777777778</v>
       </c>
@@ -704,7 +707,7 @@
         <v>322.39999999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
         <v>0.35570601851851852</v>
       </c>
@@ -724,7 +727,7 @@
         <v>312.89999999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <v>0.3562731481481482</v>
       </c>
@@ -744,7 +747,7 @@
         <v>314.5</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="9">
         <v>0.35671296296296301</v>
       </c>
@@ -764,7 +767,7 @@
         <v>312.89999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
         <v>0.35741898148148149</v>
       </c>
@@ -784,7 +787,7 @@
         <v>361.2</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="9">
         <v>0.3578587962962963</v>
       </c>
@@ -804,7 +807,7 @@
         <v>327.2</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="9">
         <v>0.35844907407407406</v>
       </c>
@@ -824,7 +827,7 @@
         <v>335.3</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="9">
         <v>0.35903935185185182</v>
       </c>
@@ -844,7 +847,7 @@
         <v>318.5</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="9">
         <v>0.35951388888888891</v>
       </c>
@@ -864,7 +867,7 @@
         <v>387.3</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="9">
         <v>0.36000000000000004</v>
       </c>
@@ -884,7 +887,7 @@
         <v>685.2</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="9">
         <v>0.3605902777777778</v>
       </c>
@@ -904,7 +907,7 @@
         <v>407.4</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="9">
         <v>0.36108796296296292</v>
       </c>
@@ -924,7 +927,7 @@
         <v>313.5</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="9">
         <v>0.36185185185185187</v>
       </c>
@@ -944,7 +947,7 @@
         <v>329.1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="9">
         <v>0.36234953703703704</v>
       </c>
@@ -964,7 +967,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="9">
         <v>0.3628703703703704</v>
       </c>
@@ -984,7 +987,7 @@
         <v>318.8</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="9">
         <v>0.36346064814814816</v>
       </c>
@@ -1004,7 +1007,7 @@
         <v>307.60000000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="9">
         <v>0.36398148148148146</v>
       </c>
@@ -1024,7 +1027,7 @@
         <v>315.60000000000002</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="9">
         <v>0.36464120370370368</v>
       </c>
@@ -1044,7 +1047,7 @@
         <v>306.7</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="9">
         <v>0.36515046296296294</v>
       </c>
@@ -1064,7 +1067,7 @@
         <v>313.39999999999998</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="9">
         <v>0.3656712962962963</v>
       </c>
@@ -1084,7 +1087,7 @@
         <v>321.89999999999998</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="9">
         <v>0.3661342592592593</v>
       </c>
@@ -1104,7 +1107,7 @@
         <v>314.7</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="9">
         <v>0.36663194444444441</v>
       </c>
@@ -1124,21 +1127,21 @@
         <v>305.3</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="9"/>
       <c r="B34" s="4"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="8">
         <v>1410</v>
       </c>
@@ -1147,7 +1150,7 @@
       </c>
       <c r="H37" s="11"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>4</v>
       </c>
@@ -1173,7 +1176,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="9">
         <v>0.36813657407407407</v>
       </c>
@@ -1196,7 +1199,7 @@
         <v>306.89999999999998</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="9">
         <v>0.36921296296296297</v>
       </c>
@@ -1217,7 +1220,7 @@
         <v>306.2</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="9">
         <v>0.36958333333333332</v>
       </c>
@@ -1238,7 +1241,7 @@
         <v>309.2</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="9">
         <v>0.36994212962962963</v>
       </c>
@@ -1259,7 +1262,7 @@
         <v>316.89999999999998</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="9">
         <v>0.37041666666666667</v>
       </c>
@@ -1280,7 +1283,7 @@
         <v>327.9</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="9">
         <v>0.3707523148148148</v>
       </c>
@@ -1301,7 +1304,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="9">
         <v>0.37123842592592587</v>
       </c>
@@ -1322,7 +1325,7 @@
         <v>346.1</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="9">
         <v>0.37170138888888887</v>
       </c>
@@ -1343,7 +1346,7 @@
         <v>489.4</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="9">
         <v>0.37208333333333332</v>
       </c>
@@ -1364,7 +1367,7 @@
         <v>660.9</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="9">
         <v>0.37248842592592596</v>
       </c>
@@ -1385,7 +1388,7 @@
         <v>655.1</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="9">
         <v>0.37283564814814812</v>
       </c>
@@ -1406,7 +1409,7 @@
         <v>486.3</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="9">
         <v>0.37321759259259263</v>
       </c>
@@ -1427,7 +1430,7 @@
         <v>352.6</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="9">
         <v>0.37354166666666666</v>
       </c>
@@ -1448,7 +1451,7 @@
         <v>313.5</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="9">
         <v>0.3739467592592593</v>
       </c>
@@ -1469,7 +1472,7 @@
         <v>324.10000000000002</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" s="9">
         <v>0.37436342592592592</v>
       </c>
@@ -1490,7 +1493,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="9">
         <v>0.3747685185185185</v>
       </c>
@@ -1511,7 +1514,7 @@
         <v>304.39999999999998</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" s="9">
         <v>0.37513888888888891</v>
       </c>
@@ -1532,7 +1535,7 @@
         <v>302.2</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" s="9">
         <v>0.37572916666666667</v>
       </c>
@@ -1555,7 +1558,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" s="9">
         <v>0.37606481481481485</v>
       </c>
@@ -1576,7 +1579,7 @@
         <v>316.10000000000002</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" s="9">
         <v>0.37643518518518521</v>
       </c>
@@ -1597,7 +1600,7 @@
         <v>321.10000000000002</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" s="9">
         <v>0.37680555555555556</v>
       </c>
@@ -1618,7 +1621,7 @@
         <v>320.3</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" s="9">
         <v>0.37731481481481483</v>
       </c>
@@ -1639,7 +1642,7 @@
         <v>316.10000000000002</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" s="9">
         <v>0.37783564814814818</v>
       </c>
@@ -1659,8 +1662,11 @@
       <c r="H61">
         <v>347</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="M61" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" s="9">
         <v>0.37820601851851854</v>
       </c>
@@ -1681,7 +1687,7 @@
         <v>435.5</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" s="9">
         <v>0.3785648148148148</v>
       </c>
@@ -1702,7 +1708,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" s="9">
         <v>0.3790162037037037</v>
       </c>
@@ -1723,7 +1729,7 @@
         <v>660.9</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="9">
         <v>0.37952546296296297</v>
       </c>
@@ -1744,7 +1750,7 @@
         <v>654.5</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="9">
         <v>0.37996527777777778</v>
       </c>
@@ -1765,7 +1771,7 @@
         <v>561.20000000000005</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="9">
         <v>0.38030092592592596</v>
       </c>
@@ -1786,7 +1792,7 @@
         <v>429.4</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="9">
         <v>0.38081018518518522</v>
       </c>
@@ -1807,7 +1813,7 @@
         <v>344.2</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="9">
         <v>0.38122685185185184</v>
       </c>
@@ -1828,7 +1834,7 @@
         <v>310.2</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="9">
         <v>0.38184027777777779</v>
       </c>
@@ -1849,7 +1855,7 @@
         <v>315.2</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="9">
         <v>0.38221064814814815</v>
       </c>
@@ -1870,7 +1876,7 @@
         <v>316.89999999999998</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="9">
         <v>0.3825810185185185</v>
       </c>
@@ -1891,10 +1897,10 @@
         <v>314.39999999999998</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B73" s="4"/>
     </row>
-    <row r="74" spans="1:8" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A74" s="10" t="s">
         <v>3</v>
       </c>
@@ -1906,7 +1912,7 @@
       <c r="E74" s="11"/>
       <c r="F74" s="11"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" s="13" t="s">
         <v>9</v>
       </c>
@@ -1918,7 +1924,7 @@
       <c r="E75" s="11"/>
       <c r="F75" s="11"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" s="13" t="s">
         <v>6</v>
       </c>
@@ -1934,7 +1940,7 @@
       <c r="E76" s="11"/>
       <c r="F76" s="11"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" s="11">
         <v>84</v>
       </c>
@@ -1950,7 +1956,7 @@
       <c r="E77" s="11"/>
       <c r="F77" s="11"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="11">
         <v>84</v>
       </c>
@@ -1964,7 +1970,7 @@
       <c r="E78" s="11"/>
       <c r="F78" s="11"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" s="11">
         <v>84</v>
       </c>
@@ -1978,7 +1984,7 @@
       <c r="E79" s="11"/>
       <c r="F79" s="11"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="11">
         <v>84</v>
       </c>
@@ -1992,7 +1998,7 @@
       <c r="E80" s="11"/>
       <c r="F80" s="11"/>
     </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A81" s="11">
         <v>84</v>
       </c>
@@ -2006,7 +2012,7 @@
       <c r="E81" s="11"/>
       <c r="F81" s="11"/>
     </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A82" s="11">
         <v>84</v>
       </c>
@@ -2020,7 +2026,7 @@
       <c r="E82" s="11"/>
       <c r="F82" s="11"/>
     </row>
-    <row r="83" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A83" s="11"/>
       <c r="B83" s="15"/>
       <c r="C83" s="15"/>
@@ -2028,7 +2034,7 @@
       <c r="E83" s="11"/>
       <c r="F83" s="11"/>
     </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A84" s="13" t="s">
         <v>8</v>
       </c>
@@ -2068,7 +2074,7 @@
       </c>
       <c r="T84" s="11"/>
     </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A85" s="13" t="s">
         <v>6</v>
       </c>
@@ -2130,7 +2136,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A86" s="11">
         <v>33</v>
       </c>
@@ -2168,7 +2174,7 @@
         <v>13.2</v>
       </c>
     </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A87" s="11">
         <v>38</v>
       </c>
@@ -2210,7 +2216,7 @@
         <v>15.4</v>
       </c>
     </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A88" s="11">
         <v>43</v>
       </c>
@@ -2246,7 +2252,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A89" s="11">
         <f>A88+5</f>
         <v>48</v>
@@ -2277,7 +2283,7 @@
         <v>14.9</v>
       </c>
     </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A90" s="11">
         <f t="shared" ref="A90:A100" si="2">A89+5</f>
         <v>53</v>
@@ -2308,7 +2314,7 @@
         <v>14.8</v>
       </c>
     </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A91" s="11">
         <f t="shared" si="2"/>
         <v>58</v>
@@ -2333,7 +2339,7 @@
         <v>15.8</v>
       </c>
     </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A92" s="11">
         <f t="shared" si="2"/>
         <v>63</v>
@@ -2358,7 +2364,7 @@
         <v>18.899999999999999</v>
       </c>
     </row>
-    <row r="93" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A93" s="11">
         <f t="shared" si="2"/>
         <v>68</v>
@@ -2383,7 +2389,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A94" s="11">
         <f>A93+5</f>
         <v>73</v>
@@ -2408,7 +2414,7 @@
         <v>16.399999999999999</v>
       </c>
     </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A95" s="11">
         <f t="shared" si="2"/>
         <v>78</v>
@@ -2439,7 +2445,7 @@
         <v>16.2</v>
       </c>
     </row>
-    <row r="96" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A96" s="11">
         <f t="shared" si="2"/>
         <v>83</v>
@@ -2470,7 +2476,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="97" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A97" s="11">
         <f t="shared" si="2"/>
         <v>88</v>
@@ -2507,7 +2513,7 @@
         <v>14.6</v>
       </c>
     </row>
-    <row r="98" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A98" s="11">
         <f>A97+5</f>
         <v>93</v>
@@ -2556,7 +2562,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="99" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A99" s="11">
         <f t="shared" si="2"/>
         <v>98</v>
@@ -2599,7 +2605,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="100" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A100" s="11">
         <f t="shared" si="2"/>
         <v>103</v>
@@ -2636,7 +2642,7 @@
         <v>22.2</v>
       </c>
     </row>
-    <row r="101" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A101" s="11">
         <f>A100+10</f>
         <v>113</v>
@@ -2685,7 +2691,7 @@
         <v>35.799999999999997</v>
       </c>
     </row>
-    <row r="102" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A102" s="11">
         <f t="shared" ref="A102:A110" si="3">A101+10</f>
         <v>123</v>
@@ -2734,7 +2740,7 @@
         <v>14.3</v>
       </c>
     </row>
-    <row r="103" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A103" s="11">
         <f>A102+10</f>
         <v>133</v>
@@ -2777,7 +2783,7 @@
         <v>14.9</v>
       </c>
     </row>
-    <row r="104" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A104" s="11">
         <f t="shared" si="3"/>
         <v>143</v>
@@ -2832,7 +2838,7 @@
         <v>13.9</v>
       </c>
     </row>
-    <row r="105" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A105" s="11">
         <f t="shared" si="3"/>
         <v>153</v>
@@ -2869,7 +2875,7 @@
         <v>28.4</v>
       </c>
     </row>
-    <row r="106" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A106" s="11">
         <f t="shared" si="3"/>
         <v>163</v>
@@ -2924,7 +2930,7 @@
         <v>12.3</v>
       </c>
     </row>
-    <row r="107" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A107" s="11">
         <f t="shared" si="3"/>
         <v>173</v>
@@ -2979,7 +2985,7 @@
         <v>13.8</v>
       </c>
     </row>
-    <row r="108" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A108" s="11">
         <f t="shared" si="3"/>
         <v>183</v>
@@ -3016,7 +3022,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="109" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A109" s="11">
         <f>A108+10</f>
         <v>193</v>
@@ -3047,7 +3053,7 @@
         <v>12.3</v>
       </c>
     </row>
-    <row r="110" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A110" s="11">
         <f t="shared" si="3"/>
         <v>203</v>
@@ -3108,7 +3114,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="111" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A111" s="11"/>
       <c r="B111" s="11"/>
       <c r="C111" s="11"/>
@@ -3116,7 +3122,7 @@
       <c r="E111" s="11"/>
       <c r="F111" s="11"/>
     </row>
-    <row r="112" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A112" s="11"/>
       <c r="B112" s="11"/>
       <c r="C112" s="11"/>
@@ -3124,7 +3130,7 @@
       <c r="E112" s="11"/>
       <c r="F112" s="11"/>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" s="13" t="s">
         <v>16</v>
       </c>
@@ -3142,7 +3148,7 @@
       </c>
       <c r="F113" s="11"/>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" s="11">
         <v>33</v>
       </c>
@@ -3160,7 +3166,7 @@
       </c>
       <c r="F114" s="13"/>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115" s="11">
         <v>38</v>
       </c>
@@ -3176,7 +3182,7 @@
       <c r="E115" s="11"/>
       <c r="F115" s="11"/>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116" s="11">
         <v>38</v>
       </c>
@@ -3192,7 +3198,7 @@
       <c r="E116" s="11"/>
       <c r="F116" s="11"/>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117" s="11">
         <v>43</v>
       </c>
@@ -3208,7 +3214,7 @@
       <c r="E117" s="11"/>
       <c r="F117" s="11"/>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118" s="11">
         <f>A117+5</f>
         <v>48</v>
@@ -3225,7 +3231,7 @@
       <c r="E118" s="11"/>
       <c r="F118" s="11"/>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119" s="11">
         <f t="shared" ref="A119:A127" si="4">A118+5</f>
         <v>53</v>
@@ -3242,7 +3248,7 @@
       <c r="E119" s="11"/>
       <c r="F119" s="11"/>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120" s="11">
         <f t="shared" si="4"/>
         <v>58</v>
@@ -3259,7 +3265,7 @@
       <c r="E120" s="11"/>
       <c r="F120" s="11"/>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121" s="11">
         <f t="shared" si="4"/>
         <v>63</v>
@@ -3276,7 +3282,7 @@
       <c r="E121" s="11"/>
       <c r="F121" s="11"/>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122" s="11">
         <f t="shared" si="4"/>
         <v>68</v>
@@ -3293,7 +3299,7 @@
       <c r="E122" s="11"/>
       <c r="F122" s="11"/>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123" s="11">
         <f>A122+5</f>
         <v>73</v>
@@ -3310,7 +3316,7 @@
       <c r="E123" s="11"/>
       <c r="F123" s="11"/>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124" s="11">
         <v>73</v>
       </c>
@@ -3326,7 +3332,7 @@
       <c r="E124" s="11"/>
       <c r="F124" s="11"/>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125" s="11">
         <f>A123+5</f>
         <v>78</v>
@@ -3343,7 +3349,7 @@
       <c r="E125" s="11"/>
       <c r="F125" s="11"/>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126" s="11">
         <f t="shared" si="4"/>
         <v>83</v>
@@ -3360,7 +3366,7 @@
       <c r="E126" s="11"/>
       <c r="F126" s="11"/>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127" s="11">
         <f t="shared" si="4"/>
         <v>88</v>
@@ -3377,7 +3383,7 @@
       <c r="E127" s="11"/>
       <c r="F127" s="11"/>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128" s="11">
         <v>88</v>
       </c>
@@ -3393,7 +3399,7 @@
       <c r="E128" s="11"/>
       <c r="F128" s="11"/>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129" s="17"/>
       <c r="B129" s="18"/>
       <c r="C129" s="11"/>
@@ -3401,7 +3407,7 @@
       <c r="E129" s="11"/>
       <c r="F129" s="11"/>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130" s="13" t="s">
         <v>16</v>
       </c>
@@ -3419,7 +3425,7 @@
       </c>
       <c r="F130" s="11"/>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131" s="11">
         <v>38</v>
       </c>
@@ -3437,7 +3443,7 @@
       </c>
       <c r="F131" s="11"/>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132" s="11">
         <v>43</v>
       </c>
@@ -3453,7 +3459,7 @@
       <c r="E132" s="11"/>
       <c r="F132" s="11"/>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133" s="11">
         <f>A132+5</f>
         <v>48</v>
@@ -3470,7 +3476,7 @@
       <c r="E133" s="11"/>
       <c r="F133" s="11"/>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134" s="11">
         <f t="shared" ref="A134:A142" si="5">A133+5</f>
         <v>53</v>
@@ -3487,7 +3493,7 @@
       <c r="E134" s="11"/>
       <c r="F134" s="11"/>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135" s="11">
         <f t="shared" si="5"/>
         <v>58</v>
@@ -3504,7 +3510,7 @@
       <c r="E135" s="11"/>
       <c r="F135" s="11"/>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136" s="11">
         <f t="shared" si="5"/>
         <v>63</v>
@@ -3521,7 +3527,7 @@
       <c r="E136" s="11"/>
       <c r="F136" s="11"/>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137" s="11">
         <f t="shared" si="5"/>
         <v>68</v>
@@ -3538,7 +3544,7 @@
       <c r="E137" s="11"/>
       <c r="F137" s="11"/>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138" s="11">
         <f>A137+5</f>
         <v>73</v>
@@ -3555,7 +3561,7 @@
       <c r="E138" s="11"/>
       <c r="F138" s="11"/>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139" s="11">
         <v>73</v>
       </c>
@@ -3571,7 +3577,7 @@
       <c r="E139" s="11"/>
       <c r="F139" s="11"/>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140" s="11">
         <f>A138+5</f>
         <v>78</v>
@@ -3588,7 +3594,7 @@
       <c r="E140" s="11"/>
       <c r="F140" s="11"/>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141" s="11">
         <f t="shared" si="5"/>
         <v>83</v>
@@ -3605,7 +3611,7 @@
       <c r="E141" s="11"/>
       <c r="F141" s="11"/>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142" s="11">
         <f t="shared" si="5"/>
         <v>88</v>
@@ -3622,7 +3628,7 @@
       <c r="E142" s="11"/>
       <c r="F142" s="11"/>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143" s="11">
         <v>88</v>
       </c>
@@ -3638,7 +3644,7 @@
       <c r="E143" s="11"/>
       <c r="F143" s="11"/>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144" s="11"/>
       <c r="B144" s="11"/>
       <c r="C144" s="11"/>

</xml_diff>

<commit_message>
Gauß 17.05. - 2:12 Pm
</commit_message>
<xml_diff>
--- a/Messprotokoll.xlsx
+++ b/Messprotokoll.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E70F401-E5A1-4B41-B3A6-8169B907918A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F0F559-BD05-4D85-ACBB-E0CD22A3A20A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10164" yWindow="2544" windowWidth="12084" windowHeight="7920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -556,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G35" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="O62" sqref="O62"/>
+    <sheetView tabSelected="1" topLeftCell="B35" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="Q61" sqref="Q61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1557,7 +1557,7 @@
         <v>41</v>
       </c>
       <c r="L53">
-        <v>364.68099999999998</v>
+        <v>5646.81</v>
       </c>
       <c r="M53">
         <v>4.76</v>
@@ -1632,7 +1632,7 @@
       </c>
       <c r="K56">
         <f>((((2*PI()*$L$51^2))^(1/2))^(-1))*$L$53*EXP(-((D56-$L$52)^2)/(2*$L$51^2))</f>
-        <v>8.8332990888130466E-5</v>
+        <v>1.3677696844008986E-3</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.3">
@@ -1657,7 +1657,7 @@
       </c>
       <c r="K57">
         <f t="shared" ref="K57:K72" si="2">((((2*PI()*$L$51^2))^(1/2))^(-1))*$L$53*EXP(-((D57-$L$52)^2)/(2*$L$51^2))</f>
-        <v>1.6213133063182779E-3</v>
+        <v>2.5104812675327524E-2</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.3">
@@ -1682,7 +1682,7 @@
       </c>
       <c r="K58">
         <f t="shared" si="2"/>
-        <v>2.0669291724518264E-2</v>
+        <v>0.3200483798249073</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.3">
@@ -1707,7 +1707,7 @@
       </c>
       <c r="K59">
         <f t="shared" si="2"/>
-        <v>0.18302013829500818</v>
+        <v>2.8339286859628974</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.3">
@@ -1732,7 +1732,7 @@
       </c>
       <c r="K60">
         <f t="shared" si="2"/>
-        <v>1.1256070379011827</v>
+        <v>17.429175300305687</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.3">
@@ -1757,7 +1757,7 @@
       </c>
       <c r="K61">
         <f t="shared" si="2"/>
-        <v>4.8082756493581558</v>
+        <v>74.452518830298629</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.3">
@@ -1782,7 +1782,7 @@
       </c>
       <c r="K62">
         <f t="shared" si="2"/>
-        <v>14.266142262821985</v>
+        <v>220.90044392530959</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.3">
@@ -1807,7 +1807,7 @@
       </c>
       <c r="K63">
         <f t="shared" si="2"/>
-        <v>29.399394130061161</v>
+        <v>455.22742552414496</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.3">
@@ -1832,7 +1832,7 @@
       </c>
       <c r="K64">
         <f t="shared" si="2"/>
-        <v>42.080883251442096</v>
+        <v>651.59071175376778</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.3">
@@ -1857,7 +1857,7 @@
       </c>
       <c r="K65">
         <f t="shared" si="2"/>
-        <v>41.835594954758534</v>
+        <v>647.79260763922457</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.3">
@@ -1882,7 +1882,7 @@
       </c>
       <c r="K66">
         <f t="shared" si="2"/>
-        <v>28.888280260587894</v>
+        <v>447.31321307743031</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.3">
@@ -1907,7 +1907,7 @@
       </c>
       <c r="K67">
         <f t="shared" si="2"/>
-        <v>13.85517655616554</v>
+        <v>214.53695018144941</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.3">
@@ -1932,7 +1932,7 @@
       </c>
       <c r="K68">
         <f t="shared" si="2"/>
-        <v>4.6154821570039344</v>
+        <v>71.467257134293789</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.3">
@@ -1957,7 +1957,7 @@
       </c>
       <c r="K69">
         <f t="shared" si="2"/>
-        <v>1.0679150937100179</v>
+        <v>16.535859094147124</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.3">
@@ -1982,7 +1982,7 @@
       </c>
       <c r="K70">
         <f t="shared" si="2"/>
-        <v>0.17162122976953642</v>
+        <v>2.6574251920854564</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.3">
@@ -2007,7 +2007,7 @@
       </c>
       <c r="K71">
         <f t="shared" si="2"/>
-        <v>1.9156666157909417E-2</v>
+        <v>0.29662651475438673</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.3">
@@ -2032,7 +2032,7 @@
       </c>
       <c r="K72">
         <f t="shared" si="2"/>
-        <v>1.4851950344309478E-3</v>
+        <v>2.2997123986100244E-2</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>